<commit_message>
Update Sprint 1   Data & Scripts Information .xlsx
</commit_message>
<xml_diff>
--- a/Sprint 1   Data & Scripts Information .xlsx
+++ b/Sprint 1   Data & Scripts Information .xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="102">
   <si>
     <t>Mapeamento de Dados da Organização</t>
   </si>
@@ -373,6 +373,29 @@
     <t>Relação Anual de Informações Sociais (RAIS)</t>
   </si>
   <si>
+    <t>http://dataviva.info/pt/data/</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <sz val="10.0"/>
+        <u/>
+      </rPr>
+      <t>https://github.com/R-and-D-IPGC/database-ipgc/tree/main/Inssues/Brazilian%20Cities%20Data/Economy/Employment%20and%20Income</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <sz val="10.0"/>
+        <u/>
+      </rPr>
+      <t>e</t>
+    </r>
+  </si>
+  <si>
     <t>http://dataviva.info/pt/build_graph/rais/all/all/all?view=Industries&amp;graph=tree_map</t>
   </si>
   <si>
@@ -422,6 +445,9 @@
     <t>Relação Anual de Informações Sociais (RAIS), processado por plataforma DataViva</t>
   </si>
   <si>
+    <t>https://github.com/R-and-D-IPGC/database-ipgc/tree/main/Inssues/Brazilian%20Cities%20Data/Economy/Employment%20and%20Income</t>
+  </si>
+  <si>
     <t>Ocupações</t>
   </si>
   <si>
@@ -432,6 +458,26 @@
   </si>
   <si>
     <t>Gráfico Treemap</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <sz val="10.0"/>
+        <u/>
+      </rPr>
+      <t>http://dataviva.info/pt/data/</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <sz val="10.0"/>
+        <u/>
+      </rPr>
+      <t>/</t>
+    </r>
   </si>
   <si>
     <t>http://dataviva.info/pt/location/4sp090607/wages?menu=new-api-jobs-occupation-tree_map&amp;url=rais%2Foccupation_family%2Fjobs%3Fcount%3Destablishment%26year%3D2017%26id_ibge%3D3550308</t>
@@ -822,8 +868,8 @@
     <xf borderId="1" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf borderId="4" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
@@ -1584,8 +1630,12 @@
       <c r="J12" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="K12" s="26"/>
-      <c r="L12" s="38"/>
+      <c r="K12" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="L12" s="27" t="s">
+        <v>74</v>
+      </c>
       <c r="M12" s="28"/>
       <c r="N12" s="20" t="s">
         <v>25</v>
@@ -1593,7 +1643,7 @@
       <c r="O12" s="16"/>
       <c r="P12" s="21"/>
       <c r="Q12" s="39" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
@@ -1601,10 +1651,10 @@
         <v>64</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D13" s="40" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>20</v>
@@ -1616,13 +1666,13 @@
         <v>21</v>
       </c>
       <c r="J13" s="16" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K13" s="17" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L13" s="18" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M13" s="19"/>
       <c r="N13" s="20" t="s">
@@ -1641,10 +1691,10 @@
         <v>64</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
@@ -1654,10 +1704,14 @@
         <v>21</v>
       </c>
       <c r="J14" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="K14" s="26"/>
-      <c r="L14" s="38"/>
+        <v>83</v>
+      </c>
+      <c r="K14" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="L14" s="27" t="s">
+        <v>84</v>
+      </c>
       <c r="M14" s="28"/>
       <c r="N14" s="20" t="s">
         <v>25</v>
@@ -1671,16 +1725,16 @@
         <v>64</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="G15" s="16"/>
       <c r="H15" s="25"/>
@@ -1688,8 +1742,12 @@
       <c r="J15" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="K15" s="26"/>
-      <c r="L15" s="38"/>
+      <c r="K15" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="L15" s="27" t="s">
+        <v>84</v>
+      </c>
       <c r="M15" s="28"/>
       <c r="N15" s="20" t="s">
         <v>25</v>
@@ -1697,25 +1755,25 @@
       <c r="O15" s="16"/>
       <c r="P15" s="23"/>
       <c r="Q15" s="39" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="B16" s="14" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
       <c r="H16" s="16"/>
       <c r="I16" s="16" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="J16" s="16"/>
       <c r="K16" s="41"/>
@@ -1725,7 +1783,7 @@
         <v>25</v>
       </c>
       <c r="O16" s="16" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="P16" s="21" t="s">
         <v>27</v>
@@ -1734,20 +1792,20 @@
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="B17" s="14" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E17" s="16"/>
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
       <c r="H17" s="16"/>
       <c r="I17" s="16" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="J17" s="16"/>
       <c r="K17" s="41"/>
@@ -1757,7 +1815,7 @@
         <v>25</v>
       </c>
       <c r="O17" s="16" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="P17" s="21" t="s">
         <v>27</v>
@@ -1766,13 +1824,13 @@
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="B18" s="14" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="E18" s="15" t="s">
         <v>20</v>
@@ -1787,10 +1845,10 @@
         <v>35</v>
       </c>
       <c r="K18" s="26" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="L18" s="27" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="M18" s="28"/>
       <c r="N18" s="20" t="s">
@@ -9382,17 +9440,23 @@
     <hyperlink r:id="rId16" ref="L10"/>
     <hyperlink r:id="rId17" ref="K11"/>
     <hyperlink r:id="rId18" ref="L11"/>
-    <hyperlink r:id="rId19" ref="Q12"/>
-    <hyperlink r:id="rId20" ref="D13"/>
-    <hyperlink r:id="rId21" ref="K13"/>
-    <hyperlink r:id="rId22" ref="L13"/>
-    <hyperlink r:id="rId23" ref="Q15"/>
-    <hyperlink r:id="rId24" ref="K18"/>
-    <hyperlink r:id="rId25" ref="L18"/>
+    <hyperlink r:id="rId19" ref="K12"/>
+    <hyperlink r:id="rId20" ref="L12"/>
+    <hyperlink r:id="rId21" ref="Q12"/>
+    <hyperlink r:id="rId22" ref="D13"/>
+    <hyperlink r:id="rId23" ref="K13"/>
+    <hyperlink r:id="rId24" ref="L13"/>
+    <hyperlink r:id="rId25" ref="K14"/>
+    <hyperlink r:id="rId26" ref="L14"/>
+    <hyperlink r:id="rId27" ref="K15"/>
+    <hyperlink r:id="rId28" ref="L15"/>
+    <hyperlink r:id="rId29" ref="Q15"/>
+    <hyperlink r:id="rId30" ref="K18"/>
+    <hyperlink r:id="rId31" ref="L18"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.787401575" footer="0.0" header="0.0" left="0.511811024" right="0.511811024" top="0.787401575"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId26"/>
+  <drawing r:id="rId32"/>
 </worksheet>
 </file>
</xml_diff>